<commit_message>
Commit to add the file: PdpNavigation.java
</commit_message>
<xml_diff>
--- a/src/test/java/com/finexus/testDataProvider/TestCasesData.xlsx
+++ b/src/test/java/com/finexus/testDataProvider/TestCasesData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="570" windowWidth="14055" windowHeight="4050"/>
+    <workbookView xWindow="240" yWindow="570" windowWidth="14055" windowHeight="4050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="InputAuthorizationData" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>userName</t>
   </si>
@@ -63,13 +63,22 @@
   </si>
   <si>
     <t>https://www.everlast.com/</t>
+  </si>
+  <si>
+    <t>blubd.softtech@gmail.com</t>
+  </si>
+  <si>
+    <t>wrongId@wrong.com</t>
+  </si>
+  <si>
+    <t>everlast#123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -112,6 +121,19 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -222,7 +244,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -250,6 +272,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -463,7 +488,7 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
@@ -567,15 +592,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -590,8 +617,8 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
+      <c r="A2" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>9</v>
@@ -601,8 +628,8 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
-        <v>8</v>
+      <c r="A3" s="20" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>9</v>
@@ -613,23 +640,12 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -638,9 +654,10 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit to add the file: TopProducts.java
</commit_message>
<xml_diff>
--- a/src/test/java/com/finexus/testDataProvider/TestCasesData.xlsx
+++ b/src/test/java/com/finexus/testDataProvider/TestCasesData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>userName</t>
   </si>
@@ -66,19 +66,13 @@
   </si>
   <si>
     <t>blubd.softtech@gmail.com</t>
-  </si>
-  <si>
-    <t>wrongId@wrong.com</t>
-  </si>
-  <si>
-    <t>everlast#123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -126,12 +120,6 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -244,7 +232,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -273,8 +261,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -592,10 +578,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -627,37 +613,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit to add the file: ReturnsandExchanges.java
</commit_message>
<xml_diff>
--- a/src/test/java/com/finexus/testDataProvider/TestCasesData.xlsx
+++ b/src/test/java/com/finexus/testDataProvider/TestCasesData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>userName</t>
   </si>
@@ -66,13 +66,25 @@
   </si>
   <si>
     <t>blubd.softtech@gmail.com</t>
+  </si>
+  <si>
+    <t>wrongUser@rightpassword.com</t>
+  </si>
+  <si>
+    <t>everlast#123</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>The account sign-in was incorrect or your account is disabled temporarily.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -120,6 +132,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFE02B27"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -232,7 +250,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -261,6 +279,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -578,10 +598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -591,7 +611,7 @@
     <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,8 +621,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="17" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
@@ -610,6 +633,34 @@
         <v>9</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -617,8 +668,12 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="A4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>